<commit_message>
EURent - made working again
</commit_message>
<xml_diff>
--- a/ZwolleFrontEnd/EURent/EURent-Demo.xlsx
+++ b/ZwolleFrontEnd/EURent/EURent-Demo.xlsx
@@ -644,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O49"/>
+  <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,599 +660,649 @@
     <col min="7" max="14" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
+      <c r="C7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>8</v>
+      <c r="A13" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>16</v>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14">
+        <v>60</v>
+      </c>
+      <c r="E14">
+        <f>MAX(15,FLOOR($D14/2.1415,1))</f>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
         <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D15">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="E15">
-        <f>MAX(15,FLOOR($D15/2.1415,1))</f>
-        <v>28</v>
+        <f t="shared" ref="E15:E17" si="0">MAX(15,FLOOR($D15/2.1415,1))</f>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
         <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D16">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="E16">
-        <f t="shared" ref="E16:E18" si="0">MAX(15,FLOOR($D16/2.1415,1))</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18">
-        <v>93</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
+    <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>43</v>
+      <c r="A20" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <f>CONCATENATE($B21,"-",$C21)</f>
+        <v>AMS-DHG</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <v>61</v>
+      </c>
+      <c r="E21">
+        <f>MAX(33,FLOOR($D21*1.3,1))</f>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
-        <f>CONCATENATE($B22,"-",$C22)</f>
-        <v>AMS-DHG</v>
+        <f t="shared" ref="A22:A26" si="1">CONCATENATE($B22,"-",$C22)</f>
+        <v>AMS-RTD</v>
       </c>
       <c r="B22" t="s">
         <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E22">
-        <f>MAX(33,FLOOR($D22*1.3,1))</f>
-        <v>79</v>
+        <f t="shared" ref="E22:E26" si="2">MAX(33,FLOOR($D22*1.3,1))</f>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
-        <f t="shared" ref="A23:A27" si="1">CONCATENATE($B23,"-",$C23)</f>
-        <v>AMS-RTD</v>
+        <f t="shared" si="1"/>
+        <v>AMS-UTR</v>
       </c>
       <c r="B23" t="s">
         <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D23">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="E23">
-        <f t="shared" ref="E23:E27" si="2">MAX(33,FLOOR($D23*1.3,1))</f>
-        <v>87</v>
+        <f t="shared" si="2"/>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f t="shared" si="1"/>
-        <v>AMS-UTR</v>
+        <v>DHG-RTD</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D24">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E24">
         <f t="shared" si="2"/>
-        <v>49</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f t="shared" si="1"/>
-        <v>DHG-RTD</v>
+        <v>DHG-UTR</v>
       </c>
       <c r="B25" t="s">
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D25">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="E25">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f t="shared" si="1"/>
-        <v>DHG-UTR</v>
+        <v>RTD-UTR</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s">
         <v>20</v>
       </c>
       <c r="D26">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E26">
         <f t="shared" si="2"/>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="str">
-        <f t="shared" si="1"/>
-        <v>RTD-UTR</v>
-      </c>
-      <c r="B27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27">
-        <v>56</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="2"/>
         <v>72</v>
       </c>
     </row>
+    <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="29" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>42</v>
+      <c r="A29" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
       </c>
-      <c r="C31" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C34" t="s">
         <v>19</v>
       </c>
+      <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C35" t="s">
         <v>19</v>
       </c>
-      <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
         <v>32</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" s="3">
+        <v>41756</v>
+      </c>
+      <c r="D47" s="3">
+        <v>41772</v>
+      </c>
+      <c r="E47" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" t="s">
+        <v>20</v>
+      </c>
+      <c r="G47" t="s">
         <v>53</v>
       </c>
-      <c r="B38" t="s">
-        <v>30</v>
-      </c>
-      <c r="C38" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="H47" t="s">
+        <v>78</v>
+      </c>
+      <c r="I47" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L46" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="M46" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="N46" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="O46" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L47" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M47" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N47" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="O47" s="1" t="s">
-        <v>7</v>
+      <c r="J47" t="s">
+        <v>76</v>
+      </c>
+      <c r="K47" t="s">
+        <v>79</v>
+      </c>
+      <c r="L47" t="s">
+        <v>79</v>
+      </c>
+      <c r="M47" t="str">
+        <f>$G47</f>
+        <v>3-RTD-18</v>
+      </c>
+      <c r="N47" s="3">
+        <v>41769</v>
+      </c>
+      <c r="O47" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="B48" t="s">
         <v>30</v>
       </c>
-      <c r="C48" s="3">
-        <v>41756</v>
-      </c>
-      <c r="D48" s="3">
-        <v>41772</v>
+      <c r="C48" s="3" t="str">
+        <f ca="1">TEXT((TODAY()-14),"DD-MM-JJJJ")</f>
+        <v>21-10-2016</v>
+      </c>
+      <c r="D48" s="3" t="str">
+        <f ca="1">TEXT((TODAY()-14),"DD-MM-JJJJ")</f>
+        <v>21-10-2016</v>
       </c>
       <c r="E48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G48" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H48" t="s">
         <v>78</v>
@@ -1269,57 +1319,7 @@
       <c r="L48" t="s">
         <v>79</v>
       </c>
-      <c r="M48" t="str">
-        <f>$G48</f>
-        <v>3-RTD-18</v>
-      </c>
-      <c r="N48" s="3">
-        <v>41769</v>
-      </c>
-      <c r="O48" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>80</v>
-      </c>
-      <c r="B49" t="s">
-        <v>30</v>
-      </c>
-      <c r="C49" s="3" t="str">
-        <f ca="1">TEXT((TODAY()-14),"DD-MM-JJJJ")</f>
-        <v>05-06-2014</v>
-      </c>
-      <c r="D49" s="3" t="str">
-        <f ca="1">TEXT((TODAY()-14),"DD-MM-JJJJ")</f>
-        <v>05-06-2014</v>
-      </c>
-      <c r="E49" t="s">
-        <v>17</v>
-      </c>
-      <c r="F49" t="s">
-        <v>19</v>
-      </c>
-      <c r="G49" t="s">
-        <v>47</v>
-      </c>
-      <c r="H49" t="s">
-        <v>78</v>
-      </c>
-      <c r="I49" t="s">
-        <v>77</v>
-      </c>
-      <c r="J49" t="s">
-        <v>76</v>
-      </c>
-      <c r="K49" t="s">
-        <v>79</v>
-      </c>
-      <c r="L49" t="s">
-        <v>79</v>
-      </c>
-      <c r="N49" s="3"/>
+      <c r="N48" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>